<commit_message>
Added iphone 14 date
</commit_message>
<xml_diff>
--- a/iphone-dates-2019.xlsx
+++ b/iphone-dates-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bratiu/PycharmProjects/pandas-apple-stock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDFA4E9-6C9C-8E4C-8F50-9A059B2329E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095DBAAF-E21A-E04B-999F-F15CA79CFEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>iPhone XS, XS Max</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Iphone 13</t>
+  </si>
+  <si>
+    <t>Iphone 14</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,11 +169,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFEEEEEE"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFEEEEEE"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,6 +193,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -461,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,7 +532,7 @@
         <v>43764</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D19" si="0">DATE(YEAR(C3)-2019+B3, MONTH(C3), DAY(C3))</f>
+        <f t="shared" ref="D3:D17" si="0">DATE(YEAR(C3)-2019+B3, MONTH(C3), DAY(C3))</f>
         <v>43399</v>
       </c>
     </row>
@@ -757,6 +774,20 @@
       <c r="D19" s="3">
         <f>DATE(B19, MONTH(C19), DAY(C19))</f>
         <v>44463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2022</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45185</v>
+      </c>
+      <c r="D20" s="3">
+        <v>44820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added iphone 15 date
</commit_message>
<xml_diff>
--- a/iphone-dates-2019.xlsx
+++ b/iphone-dates-2019.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bratiu/PycharmProjects/pandas-apple-stock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095DBAAF-E21A-E04B-999F-F15CA79CFEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3230D9-644D-7149-9C90-536BB2CA90C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>iPhone XS, XS Max</t>
   </si>
@@ -104,6 +103,9 @@
   </si>
   <si>
     <t>Iphone 14</t>
+  </si>
+  <si>
+    <t>Iphone 15</t>
   </si>
 </sst>
 </file>
@@ -478,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -790,6 +792,23 @@
         <v>44820</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2023</v>
+      </c>
+      <c r="C21" s="5">
+        <v>45557</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>